<commit_message>
vovliendo a importar la libreria log aun sigue sin reconocerla
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javier\Desktop\reto final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8474D4E6-EEE2-4AA3-A0C0-99AAB78EB405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE59F7A-48C1-4BE7-9F2D-2DF47B8067CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -47,34 +47,55 @@
     <t>Estatus</t>
   </si>
   <si>
-    <t>puto animal</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>puto</t>
+    <t>simon</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>perro</t>
+  </si>
+  <si>
+    <t>es mi perrito</t>
+  </si>
+  <si>
+    <t>esta muy bien</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>es perro</t>
+  </si>
+  <si>
+    <t>lo quiero mucho</t>
+  </si>
+  <si>
+    <t>le falta un ojo</t>
   </si>
   <si>
     <t>pepe</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>si</t>
-  </si>
-  <si>
-    <t>hola</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>reptil</t>
+  </si>
+  <si>
+    <t>es una tortuga</t>
+  </si>
+  <si>
+    <t>esta bien</t>
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -82,14 +103,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -115,18 +129,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -438,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,119 +483,96 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2">
+      <c r="A2" t="n">
+        <v>495.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1" t="b">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>809.0</v>
+        <v>546.0</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>506.0</v>
+        <v>88.0</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>872.0</v>
+        <v>61.0</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>869.0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>